<commit_message>
Add lab3 document, add tests.
</commit_message>
<xml_diff>
--- a/Lab3/Lab03_BBT_TCs_Form.xlsx
+++ b/Lab3/Lab03_BBT_TCs_Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED8395A-87D2-40DD-96DA-22CC1B47316C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842A4176-BCA8-4DF4-B383-82216E0091E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="111">
   <si>
     <t>Condition</t>
   </si>
@@ -594,6 +594,12 @@
       </rPr>
       <t>failed</t>
     </r>
+  </si>
+  <si>
+    <t>[ary</t>
+  </si>
+  <si>
+    <t>run2</t>
   </si>
 </sst>
 </file>
@@ -1321,7 +1327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1559,6 +1565,55 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1586,61 +1641,94 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1649,22 +1737,67 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1679,144 +1812,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2634,12 +2643,12 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="22"/>
-      <c r="D1" s="97" t="s">
+      <c r="D1" s="116" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="99"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="118"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="L2" s="91" t="s">
@@ -2652,33 +2661,33 @@
       <c r="Q2" s="92"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="L3" s="100" t="s">
+      <c r="L3" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="M3" s="101"/>
-      <c r="N3" s="102" t="s">
+      <c r="M3" s="120"/>
+      <c r="N3" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="O3" s="103"/>
-      <c r="P3" s="103"/>
-      <c r="Q3" s="104"/>
+      <c r="O3" s="122"/>
+      <c r="P3" s="122"/>
+      <c r="Q3" s="123"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
-      <c r="L4" s="105" t="s">
+      <c r="L4" s="124" t="s">
         <v>49</v>
       </c>
-      <c r="M4" s="105"/>
+      <c r="M4" s="124"/>
       <c r="N4" s="75" t="s">
         <v>52</v>
       </c>
       <c r="O4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="P4" s="102">
+      <c r="P4" s="121">
         <v>1211</v>
       </c>
-      <c r="Q4" s="104"/>
+      <c r="Q4" s="123"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
@@ -2833,12 +2842,12 @@
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B1" s="22"/>
-      <c r="D1" s="97" t="s">
+      <c r="D1" s="116" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="99"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="118"/>
     </row>
     <row r="2" spans="2:17" s="66" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="22"/>
@@ -2858,49 +2867,49 @@
       <c r="H3" s="90"/>
     </row>
     <row r="5" spans="2:17" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="118" t="s">
+      <c r="B5" s="127" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="118"/>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
-      <c r="H5" s="119" t="s">
+      <c r="C5" s="127"/>
+      <c r="D5" s="127"/>
+      <c r="E5" s="127"/>
+      <c r="H5" s="128" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="128"/>
     </row>
     <row r="6" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="118"/>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
+      <c r="B6" s="127"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
       <c r="F6" s="66"/>
       <c r="G6" s="66"/>
-      <c r="H6" s="120"/>
-      <c r="I6" s="120"/>
-      <c r="J6" s="120"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="129"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="G7" s="121" t="s">
+      <c r="G7" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="123" t="s">
+      <c r="H7" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="112" t="s">
+      <c r="I7" s="141" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="113"/>
-      <c r="K7" s="113"/>
-      <c r="L7" s="113"/>
-      <c r="M7" s="113"/>
-      <c r="N7" s="113"/>
-      <c r="O7" s="114"/>
-      <c r="P7" s="115" t="s">
+      <c r="J7" s="142"/>
+      <c r="K7" s="142"/>
+      <c r="L7" s="142"/>
+      <c r="M7" s="142"/>
+      <c r="N7" s="142"/>
+      <c r="O7" s="143"/>
+      <c r="P7" s="144" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="115"/>
+      <c r="Q7" s="144"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
@@ -2915,8 +2924,8 @@
       <c r="E8" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="122"/>
-      <c r="H8" s="124"/>
+      <c r="G8" s="131"/>
+      <c r="H8" s="133"/>
       <c r="I8" s="14" t="s">
         <v>67</v>
       </c>
@@ -2932,30 +2941,30 @@
       <c r="M8" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="N8" s="112" t="s">
+      <c r="N8" s="141" t="s">
         <v>72</v>
       </c>
-      <c r="O8" s="114"/>
-      <c r="P8" s="112" t="s">
+      <c r="O8" s="143"/>
+      <c r="P8" s="141" t="s">
         <v>7</v>
       </c>
-      <c r="Q8" s="114"/>
+      <c r="Q8" s="143"/>
     </row>
     <row r="9" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="84">
         <v>1</v>
       </c>
-      <c r="C9" s="154" t="s">
+      <c r="C9" s="134" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="158" t="s">
+      <c r="D9" s="98" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="159"/>
+      <c r="E9" s="99"/>
       <c r="G9" s="21">
         <v>1</v>
       </c>
-      <c r="H9" s="161" t="s">
+      <c r="H9" s="101" t="s">
         <v>61</v>
       </c>
       <c r="I9" s="20">
@@ -2967,28 +2976,28 @@
       <c r="K9" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="L9" s="162" t="s">
+      <c r="L9" s="102" t="s">
         <v>73</v>
       </c>
       <c r="M9" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="N9" s="106" t="s">
+      <c r="N9" s="137" t="s">
         <v>78</v>
       </c>
-      <c r="O9" s="107"/>
-      <c r="P9" s="110" t="s">
+      <c r="O9" s="138"/>
+      <c r="P9" s="139" t="s">
         <v>79</v>
       </c>
-      <c r="Q9" s="111"/>
+      <c r="Q9" s="140"/>
     </row>
     <row r="10" spans="2:17" s="66" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="84">
         <v>2</v>
       </c>
-      <c r="C10" s="157"/>
-      <c r="D10" s="158"/>
-      <c r="E10" s="159" t="s">
+      <c r="C10" s="135"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="99" t="s">
         <v>56</v>
       </c>
       <c r="G10" s="21">
@@ -3006,7 +3015,7 @@
       <c r="K10" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="L10" s="162" t="s">
+      <c r="L10" s="102" t="s">
         <v>73</v>
       </c>
       <c r="M10" s="38" t="s">
@@ -3016,7 +3025,7 @@
         <v>78</v>
       </c>
       <c r="O10" s="94"/>
-      <c r="P10" s="164" t="s">
+      <c r="P10" s="103" t="s">
         <v>81</v>
       </c>
       <c r="Q10" s="95"/>
@@ -3025,9 +3034,9 @@
       <c r="B11" s="84">
         <v>3</v>
       </c>
-      <c r="C11" s="157"/>
-      <c r="D11" s="156"/>
-      <c r="E11" s="159" t="s">
+      <c r="C11" s="135"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="99" t="s">
         <v>58</v>
       </c>
       <c r="G11" s="21">
@@ -3055,7 +3064,7 @@
         <v>78</v>
       </c>
       <c r="O11" s="94"/>
-      <c r="P11" s="164" t="s">
+      <c r="P11" s="103" t="s">
         <v>81</v>
       </c>
       <c r="Q11" s="95"/>
@@ -3064,9 +3073,9 @@
       <c r="B12" s="84">
         <v>4</v>
       </c>
-      <c r="C12" s="155"/>
+      <c r="C12" s="136"/>
       <c r="D12" s="84"/>
-      <c r="E12" s="159" t="s">
+      <c r="E12" s="99" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="21">
@@ -3084,32 +3093,32 @@
       <c r="K12" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="L12" s="162" t="s">
+      <c r="L12" s="102" t="s">
         <v>82</v>
       </c>
       <c r="M12" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="N12" s="106" t="s">
+      <c r="N12" s="137" t="s">
         <v>78</v>
       </c>
-      <c r="O12" s="107"/>
-      <c r="P12" s="163" t="s">
+      <c r="O12" s="138"/>
+      <c r="P12" s="145" t="s">
         <v>81</v>
       </c>
-      <c r="Q12" s="174"/>
+      <c r="Q12" s="146"/>
     </row>
     <row r="13" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="84">
         <v>5</v>
       </c>
-      <c r="C13" s="154" t="s">
+      <c r="C13" s="134" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="158" t="s">
+      <c r="D13" s="98" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="160" t="s">
+      <c r="E13" s="100" t="s">
         <v>62</v>
       </c>
       <c r="G13" s="21">
@@ -3127,28 +3136,28 @@
       <c r="K13" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="L13" s="162" t="s">
+      <c r="L13" s="102" t="s">
         <v>93</v>
       </c>
       <c r="M13" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="N13" s="106" t="s">
+      <c r="N13" s="137" t="s">
         <v>78</v>
       </c>
-      <c r="O13" s="107"/>
-      <c r="P13" s="163" t="s">
+      <c r="O13" s="138"/>
+      <c r="P13" s="145" t="s">
         <v>81</v>
       </c>
-      <c r="Q13" s="107"/>
+      <c r="Q13" s="138"/>
     </row>
     <row r="14" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="84">
         <v>6</v>
       </c>
-      <c r="C14" s="155"/>
+      <c r="C14" s="136"/>
       <c r="D14" s="84"/>
-      <c r="E14" s="159"/>
+      <c r="E14" s="99"/>
       <c r="G14" s="21">
         <v>6</v>
       </c>
@@ -3158,16 +3167,16 @@
       <c r="K14" s="20"/>
       <c r="L14" s="38"/>
       <c r="M14" s="20"/>
-      <c r="N14" s="106"/>
-      <c r="O14" s="107"/>
-      <c r="P14" s="106"/>
-      <c r="Q14" s="107"/>
+      <c r="N14" s="137"/>
+      <c r="O14" s="138"/>
+      <c r="P14" s="137"/>
+      <c r="Q14" s="138"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="84">
         <v>7</v>
       </c>
-      <c r="C15" s="116"/>
+      <c r="C15" s="125"/>
       <c r="D15" s="84"/>
       <c r="E15" s="84"/>
       <c r="G15" s="21">
@@ -3179,16 +3188,16 @@
       <c r="K15" s="20"/>
       <c r="L15" s="38"/>
       <c r="M15" s="20"/>
-      <c r="N15" s="106"/>
-      <c r="O15" s="107"/>
-      <c r="P15" s="106"/>
-      <c r="Q15" s="107"/>
+      <c r="N15" s="137"/>
+      <c r="O15" s="138"/>
+      <c r="P15" s="137"/>
+      <c r="Q15" s="138"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="84">
         <v>8</v>
       </c>
-      <c r="C16" s="117"/>
+      <c r="C16" s="126"/>
       <c r="D16" s="84"/>
       <c r="E16" s="84"/>
       <c r="G16" s="21">
@@ -3200,16 +3209,16 @@
       <c r="K16" s="20"/>
       <c r="L16" s="38"/>
       <c r="M16" s="20"/>
-      <c r="N16" s="106"/>
-      <c r="O16" s="107"/>
-      <c r="P16" s="106"/>
-      <c r="Q16" s="107"/>
+      <c r="N16" s="137"/>
+      <c r="O16" s="138"/>
+      <c r="P16" s="137"/>
+      <c r="Q16" s="138"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B17" s="84">
         <v>9</v>
       </c>
-      <c r="C17" s="116"/>
+      <c r="C17" s="125"/>
       <c r="D17" s="84"/>
       <c r="E17" s="84"/>
       <c r="G17" s="21">
@@ -3221,16 +3230,16 @@
       <c r="K17" s="20"/>
       <c r="L17" s="38"/>
       <c r="M17" s="20"/>
-      <c r="N17" s="106"/>
-      <c r="O17" s="107"/>
-      <c r="P17" s="110"/>
-      <c r="Q17" s="111"/>
+      <c r="N17" s="137"/>
+      <c r="O17" s="138"/>
+      <c r="P17" s="139"/>
+      <c r="Q17" s="140"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B18" s="84">
         <v>10</v>
       </c>
-      <c r="C18" s="117"/>
+      <c r="C18" s="126"/>
       <c r="D18" s="84"/>
       <c r="E18" s="84"/>
       <c r="G18" s="21"/>
@@ -3240,16 +3249,16 @@
       <c r="K18" s="20"/>
       <c r="L18" s="38"/>
       <c r="M18" s="20"/>
-      <c r="N18" s="106"/>
-      <c r="O18" s="107"/>
-      <c r="P18" s="106"/>
-      <c r="Q18" s="107"/>
+      <c r="N18" s="137"/>
+      <c r="O18" s="138"/>
+      <c r="P18" s="137"/>
+      <c r="Q18" s="138"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B19" s="84">
         <v>11</v>
       </c>
-      <c r="C19" s="116"/>
+      <c r="C19" s="125"/>
       <c r="D19" s="84"/>
       <c r="E19" s="84"/>
       <c r="G19" s="11"/>
@@ -3259,16 +3268,16 @@
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
-      <c r="N19" s="106"/>
-      <c r="O19" s="107"/>
-      <c r="P19" s="108"/>
-      <c r="Q19" s="109"/>
+      <c r="N19" s="137"/>
+      <c r="O19" s="138"/>
+      <c r="P19" s="147"/>
+      <c r="Q19" s="148"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B20" s="84">
         <v>12</v>
       </c>
-      <c r="C20" s="117"/>
+      <c r="C20" s="126"/>
       <c r="D20" s="84"/>
       <c r="E20" s="84"/>
       <c r="G20" s="11"/>
@@ -3278,16 +3287,16 @@
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
-      <c r="N20" s="106"/>
-      <c r="O20" s="107"/>
-      <c r="P20" s="108"/>
-      <c r="Q20" s="109"/>
+      <c r="N20" s="137"/>
+      <c r="O20" s="138"/>
+      <c r="P20" s="147"/>
+      <c r="Q20" s="148"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B21" s="84">
         <v>13</v>
       </c>
-      <c r="C21" s="116"/>
+      <c r="C21" s="125"/>
       <c r="D21" s="84"/>
       <c r="E21" s="84"/>
       <c r="G21" s="11"/>
@@ -3297,16 +3306,16 @@
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
-      <c r="N21" s="106"/>
-      <c r="O21" s="107"/>
-      <c r="P21" s="108"/>
-      <c r="Q21" s="109"/>
+      <c r="N21" s="137"/>
+      <c r="O21" s="138"/>
+      <c r="P21" s="147"/>
+      <c r="Q21" s="148"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B22" s="84">
         <v>14</v>
       </c>
-      <c r="C22" s="117"/>
+      <c r="C22" s="126"/>
       <c r="D22" s="84"/>
       <c r="E22" s="84"/>
       <c r="G22" s="14"/>
@@ -3316,16 +3325,16 @@
       <c r="K22" s="20"/>
       <c r="L22" s="38"/>
       <c r="M22" s="20"/>
-      <c r="N22" s="106"/>
-      <c r="O22" s="107"/>
-      <c r="P22" s="108"/>
-      <c r="Q22" s="109"/>
+      <c r="N22" s="137"/>
+      <c r="O22" s="138"/>
+      <c r="P22" s="147"/>
+      <c r="Q22" s="148"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B23" s="84">
         <v>15</v>
       </c>
-      <c r="C23" s="116"/>
+      <c r="C23" s="125"/>
       <c r="D23" s="84"/>
       <c r="E23" s="84"/>
     </row>
@@ -3333,7 +3342,7 @@
       <c r="B24" s="84">
         <v>16</v>
       </c>
-      <c r="C24" s="117"/>
+      <c r="C24" s="126"/>
       <c r="D24" s="84"/>
       <c r="E24" s="84"/>
     </row>
@@ -3440,18 +3449,18 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="B5:E6"/>
-    <mergeCell ref="H5:J6"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
     <mergeCell ref="P15:Q15"/>
     <mergeCell ref="P16:Q16"/>
     <mergeCell ref="P17:Q17"/>
@@ -3468,18 +3477,18 @@
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="N13:O13"/>
     <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="B5:E6"/>
+    <mergeCell ref="H5:J6"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3495,7 +3504,7 @@
   <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15:R18"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3522,12 +3531,12 @@
       <c r="B1" s="22"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="97" t="s">
+      <c r="E1" s="116" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="99"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="118"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C2" s="77" t="s">
@@ -3544,57 +3553,57 @@
       <c r="J4" s="77"/>
     </row>
     <row r="5" spans="2:18" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="130" t="s">
+      <c r="B5" s="153" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="130"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="130"/>
-      <c r="H5" s="119" t="s">
+      <c r="C5" s="153"/>
+      <c r="D5" s="153"/>
+      <c r="E5" s="153"/>
+      <c r="H5" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119"/>
-      <c r="K5" s="119"/>
-      <c r="L5" s="119"/>
-      <c r="M5" s="119"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="128"/>
+      <c r="K5" s="128"/>
+      <c r="L5" s="128"/>
+      <c r="M5" s="128"/>
     </row>
     <row r="6" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="131"/>
-      <c r="C6" s="131"/>
-      <c r="D6" s="131"/>
-      <c r="E6" s="131"/>
+      <c r="B6" s="154"/>
+      <c r="C6" s="154"/>
+      <c r="D6" s="154"/>
+      <c r="E6" s="154"/>
       <c r="F6" s="66"/>
       <c r="G6" s="66"/>
-      <c r="H6" s="119"/>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
+      <c r="H6" s="128"/>
+      <c r="I6" s="128"/>
+      <c r="J6" s="128"/>
+      <c r="K6" s="128"/>
+      <c r="L6" s="128"/>
+      <c r="M6" s="128"/>
     </row>
     <row r="7" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F7" s="5"/>
-      <c r="H7" s="121" t="s">
+      <c r="H7" s="130" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="121" t="s">
+      <c r="I7" s="130" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="121" t="s">
+      <c r="J7" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="123" t="s">
+      <c r="K7" s="132" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="127" t="s">
+      <c r="L7" s="150" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="128"/>
-      <c r="N7" s="128"/>
-      <c r="O7" s="128"/>
-      <c r="P7" s="128"/>
-      <c r="Q7" s="129"/>
+      <c r="M7" s="151"/>
+      <c r="N7" s="151"/>
+      <c r="O7" s="151"/>
+      <c r="P7" s="151"/>
+      <c r="Q7" s="152"/>
       <c r="R7" s="86" t="s">
         <v>6</v>
       </c>
@@ -3606,15 +3615,15 @@
       <c r="C8" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="112" t="s">
+      <c r="D8" s="141" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="114"/>
+      <c r="E8" s="143"/>
       <c r="F8" s="3"/>
-      <c r="H8" s="122"/>
-      <c r="I8" s="122"/>
-      <c r="J8" s="122"/>
-      <c r="K8" s="124"/>
+      <c r="H8" s="131"/>
+      <c r="I8" s="131"/>
+      <c r="J8" s="131"/>
+      <c r="K8" s="133"/>
       <c r="L8" s="30" t="s">
         <v>67</v>
       </c>
@@ -3638,10 +3647,10 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="116" t="s">
+      <c r="B9" s="125" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="154" t="s">
+      <c r="C9" s="134" t="s">
         <v>55</v>
       </c>
       <c r="D9" s="84">
@@ -3672,7 +3681,7 @@
       <c r="N9" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="O9" s="167" t="s">
+      <c r="O9" s="106" t="s">
         <v>82</v>
       </c>
       <c r="P9" s="71" t="s">
@@ -3681,17 +3690,17 @@
       <c r="Q9" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="R9" s="166" t="s">
+      <c r="R9" s="105" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="132"/>
-      <c r="C10" s="157"/>
+      <c r="B10" s="149"/>
+      <c r="C10" s="135"/>
       <c r="D10" s="84">
         <v>2</v>
       </c>
-      <c r="E10" s="161" t="s">
+      <c r="E10" s="101" t="s">
         <v>84</v>
       </c>
       <c r="F10" s="3"/>
@@ -3716,7 +3725,7 @@
       <c r="N10" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="O10" s="167" t="s">
+      <c r="O10" s="106" t="s">
         <v>73</v>
       </c>
       <c r="P10" s="71" t="s">
@@ -3725,13 +3734,13 @@
       <c r="Q10" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="R10" s="168" t="s">
+      <c r="R10" s="107" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="132"/>
-      <c r="C11" s="157"/>
+      <c r="B11" s="149"/>
+      <c r="C11" s="135"/>
       <c r="D11" s="84">
         <v>3</v>
       </c>
@@ -3760,7 +3769,7 @@
       <c r="N11" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="O11" s="167" t="s">
+      <c r="O11" s="106" t="s">
         <v>93</v>
       </c>
       <c r="P11" s="71" t="s">
@@ -3769,13 +3778,13 @@
       <c r="Q11" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="R11" s="165" t="s">
+      <c r="R11" s="104" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="132"/>
-      <c r="C12" s="157"/>
+      <c r="B12" s="149"/>
+      <c r="C12" s="135"/>
       <c r="D12" s="84">
         <v>4</v>
       </c>
@@ -3798,8 +3807,8 @@
       <c r="R12" s="71"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="132"/>
-      <c r="C13" s="157"/>
+      <c r="B13" s="149"/>
+      <c r="C13" s="135"/>
       <c r="D13" s="84">
         <v>5</v>
       </c>
@@ -3822,8 +3831,8 @@
       <c r="R13" s="71"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="117"/>
-      <c r="C14" s="155"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="136"/>
       <c r="D14" s="84">
         <v>6</v>
       </c>
@@ -3846,10 +3855,10 @@
       <c r="R14" s="71"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B15" s="116" t="s">
+      <c r="B15" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="154" t="s">
+      <c r="C15" s="134" t="s">
         <v>60</v>
       </c>
       <c r="D15" s="84">
@@ -3865,7 +3874,7 @@
       <c r="I15" s="71">
         <v>7</v>
       </c>
-      <c r="J15" s="167" t="s">
+      <c r="J15" s="106" t="s">
         <v>100</v>
       </c>
       <c r="K15" s="71" t="s">
@@ -3877,10 +3886,10 @@
       <c r="M15" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="N15" s="167" t="s">
+      <c r="N15" s="106" t="s">
         <v>95</v>
       </c>
-      <c r="O15" s="167" t="s">
+      <c r="O15" s="106" t="s">
         <v>73</v>
       </c>
       <c r="P15" s="71" t="s">
@@ -3889,17 +3898,17 @@
       <c r="Q15" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="R15" s="166" t="s">
+      <c r="R15" s="105" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B16" s="132"/>
-      <c r="C16" s="157"/>
+      <c r="B16" s="149"/>
+      <c r="C16" s="135"/>
       <c r="D16" s="84">
         <v>8</v>
       </c>
-      <c r="E16" s="161" t="s">
+      <c r="E16" s="101" t="s">
         <v>87</v>
       </c>
       <c r="F16" s="3"/>
@@ -3909,7 +3918,7 @@
       <c r="I16" s="71">
         <v>8</v>
       </c>
-      <c r="J16" s="167" t="s">
+      <c r="J16" s="106" t="s">
         <v>100</v>
       </c>
       <c r="K16" s="71" t="s">
@@ -3924,7 +3933,7 @@
       <c r="N16" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="O16" s="167" t="s">
+      <c r="O16" s="106" t="s">
         <v>73</v>
       </c>
       <c r="P16" s="71" t="s">
@@ -3933,17 +3942,17 @@
       <c r="Q16" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="R16" s="168" t="s">
+      <c r="R16" s="107" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B17" s="132"/>
-      <c r="C17" s="157"/>
+      <c r="B17" s="149"/>
+      <c r="C17" s="135"/>
       <c r="D17" s="84">
         <v>9</v>
       </c>
-      <c r="E17" s="161" t="s">
+      <c r="E17" s="101" t="s">
         <v>88</v>
       </c>
       <c r="F17" s="3"/>
@@ -3953,7 +3962,7 @@
       <c r="I17" s="71">
         <v>9</v>
       </c>
-      <c r="J17" s="167" t="s">
+      <c r="J17" s="106" t="s">
         <v>100</v>
       </c>
       <c r="K17" s="71" t="s">
@@ -3968,7 +3977,7 @@
       <c r="N17" s="71" t="s">
         <v>98</v>
       </c>
-      <c r="O17" s="167" t="s">
+      <c r="O17" s="106" t="s">
         <v>73</v>
       </c>
       <c r="P17" s="71" t="s">
@@ -3977,13 +3986,13 @@
       <c r="Q17" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="R17" s="168" t="s">
+      <c r="R17" s="107" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B18" s="132"/>
-      <c r="C18" s="157"/>
+      <c r="B18" s="149"/>
+      <c r="C18" s="135"/>
       <c r="D18" s="84">
         <v>10</v>
       </c>
@@ -3997,7 +4006,7 @@
       <c r="I18" s="71">
         <v>10</v>
       </c>
-      <c r="J18" s="167" t="s">
+      <c r="J18" s="106" t="s">
         <v>100</v>
       </c>
       <c r="K18" s="71" t="s">
@@ -4009,10 +4018,10 @@
       <c r="M18" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="N18" s="167" t="s">
+      <c r="N18" s="106" t="s">
         <v>99</v>
       </c>
-      <c r="O18" s="167" t="s">
+      <c r="O18" s="106" t="s">
         <v>73</v>
       </c>
       <c r="P18" s="71" t="s">
@@ -4021,13 +4030,13 @@
       <c r="Q18" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="R18" s="165" t="s">
+      <c r="R18" s="104" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B19" s="132"/>
-      <c r="C19" s="157"/>
+      <c r="B19" s="149"/>
+      <c r="C19" s="135"/>
       <c r="D19" s="84">
         <v>11</v>
       </c>
@@ -4050,8 +4059,8 @@
       <c r="R19" s="71"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B20" s="117"/>
-      <c r="C20" s="155"/>
+      <c r="B20" s="126"/>
+      <c r="C20" s="136"/>
       <c r="D20" s="84">
         <v>12</v>
       </c>
@@ -4074,10 +4083,10 @@
       <c r="R20" s="72"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B21" s="116" t="s">
+      <c r="B21" s="125" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="116"/>
+      <c r="C21" s="125"/>
       <c r="D21" s="84">
         <v>13</v>
       </c>
@@ -4100,8 +4109,8 @@
       <c r="R21" s="72"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B22" s="132"/>
-      <c r="C22" s="132"/>
+      <c r="B22" s="149"/>
+      <c r="C22" s="149"/>
       <c r="D22" s="84">
         <v>14</v>
       </c>
@@ -4124,8 +4133,8 @@
       <c r="R22" s="72"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B23" s="132"/>
-      <c r="C23" s="132"/>
+      <c r="B23" s="149"/>
+      <c r="C23" s="149"/>
       <c r="D23" s="84">
         <v>15</v>
       </c>
@@ -4148,8 +4157,8 @@
       <c r="R23" s="71"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B24" s="132"/>
-      <c r="C24" s="132"/>
+      <c r="B24" s="149"/>
+      <c r="C24" s="149"/>
       <c r="D24" s="84">
         <v>16</v>
       </c>
@@ -4172,8 +4181,8 @@
       <c r="R24" s="71"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B25" s="132"/>
-      <c r="C25" s="132"/>
+      <c r="B25" s="149"/>
+      <c r="C25" s="149"/>
       <c r="D25" s="84">
         <v>17</v>
       </c>
@@ -4196,8 +4205,8 @@
       <c r="R25" s="71"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B26" s="117"/>
-      <c r="C26" s="117"/>
+      <c r="B26" s="126"/>
+      <c r="C26" s="126"/>
       <c r="D26" s="84">
         <v>18</v>
       </c>
@@ -4220,10 +4229,10 @@
       <c r="R26" s="72"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B27" s="116" t="s">
+      <c r="B27" s="125" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="116"/>
+      <c r="C27" s="125"/>
       <c r="D27" s="84">
         <v>19</v>
       </c>
@@ -4247,8 +4256,8 @@
       <c r="S27" s="3"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B28" s="132"/>
-      <c r="C28" s="132"/>
+      <c r="B28" s="149"/>
+      <c r="C28" s="149"/>
       <c r="D28" s="84">
         <v>20</v>
       </c>
@@ -4272,8 +4281,8 @@
       <c r="S28" s="3"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B29" s="132"/>
-      <c r="C29" s="132"/>
+      <c r="B29" s="149"/>
+      <c r="C29" s="149"/>
       <c r="D29" s="84">
         <v>21</v>
       </c>
@@ -4297,8 +4306,8 @@
       <c r="S29" s="3"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B30" s="132"/>
-      <c r="C30" s="132"/>
+      <c r="B30" s="149"/>
+      <c r="C30" s="149"/>
       <c r="D30" s="84">
         <v>22</v>
       </c>
@@ -4322,8 +4331,8 @@
       <c r="S30" s="3"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B31" s="132"/>
-      <c r="C31" s="132"/>
+      <c r="B31" s="149"/>
+      <c r="C31" s="149"/>
       <c r="D31" s="84">
         <v>23</v>
       </c>
@@ -4346,8 +4355,8 @@
       <c r="R31" s="71"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B32" s="117"/>
-      <c r="C32" s="117"/>
+      <c r="B32" s="126"/>
+      <c r="C32" s="126"/>
       <c r="D32" s="84">
         <v>24</v>
       </c>
@@ -4369,10 +4378,10 @@
       <c r="R32" s="72"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B33" s="116" t="s">
+      <c r="B33" s="125" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="116"/>
+      <c r="C33" s="125"/>
       <c r="D33" s="84">
         <v>25</v>
       </c>
@@ -4394,8 +4403,8 @@
       <c r="R33" s="87"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B34" s="132"/>
-      <c r="C34" s="132"/>
+      <c r="B34" s="149"/>
+      <c r="C34" s="149"/>
       <c r="D34" s="84">
         <v>26</v>
       </c>
@@ -4417,8 +4426,8 @@
       <c r="R34" s="72"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B35" s="132"/>
-      <c r="C35" s="132"/>
+      <c r="B35" s="149"/>
+      <c r="C35" s="149"/>
       <c r="D35" s="84">
         <v>27</v>
       </c>
@@ -4440,8 +4449,8 @@
       <c r="R35" s="71"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B36" s="132"/>
-      <c r="C36" s="132"/>
+      <c r="B36" s="149"/>
+      <c r="C36" s="149"/>
       <c r="D36" s="84">
         <v>28</v>
       </c>
@@ -4463,8 +4472,8 @@
       <c r="R36" s="71"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B37" s="132"/>
-      <c r="C37" s="132"/>
+      <c r="B37" s="149"/>
+      <c r="C37" s="149"/>
       <c r="D37" s="84">
         <v>29</v>
       </c>
@@ -4486,8 +4495,8 @@
       <c r="R37" s="71"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B38" s="117"/>
-      <c r="C38" s="117"/>
+      <c r="B38" s="126"/>
+      <c r="C38" s="126"/>
       <c r="D38" s="84">
         <v>30</v>
       </c>
@@ -4512,8 +4521,8 @@
       <c r="A40" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="H40" s="125"/>
-      <c r="I40" s="126"/>
+      <c r="H40" s="155"/>
+      <c r="I40" s="156"/>
       <c r="J40" s="66"/>
       <c r="K40" s="66"/>
       <c r="L40" s="66"/>
@@ -4550,6 +4559,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="L7:Q7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B5:E6"/>
+    <mergeCell ref="H5:M6"/>
     <mergeCell ref="B27:B32"/>
     <mergeCell ref="C27:C32"/>
     <mergeCell ref="B33:B38"/>
@@ -4560,16 +4579,6 @@
     <mergeCell ref="C15:C20"/>
     <mergeCell ref="B21:B26"/>
     <mergeCell ref="C21:C26"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="L7:Q7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B5:E6"/>
-    <mergeCell ref="H5:M6"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4584,8 +4593,8 @@
   </sheetPr>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4606,12 +4615,12 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B1" s="22"/>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="116" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="99"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="118"/>
     </row>
     <row r="2" spans="2:13" s="66" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="22"/>
@@ -4622,52 +4631,55 @@
     </row>
     <row r="3" spans="2:13" s="66" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="22"/>
-      <c r="C3" s="152" t="s">
+      <c r="C3" s="184" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="152"/>
-      <c r="E3" s="152"/>
-      <c r="F3" s="152"/>
-      <c r="G3" s="152"/>
+      <c r="D3" s="184"/>
+      <c r="E3" s="184"/>
+      <c r="F3" s="184"/>
+      <c r="G3" s="184"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="153"/>
-      <c r="D4" s="153"/>
-      <c r="E4" s="153"/>
-      <c r="F4" s="153"/>
-      <c r="G4" s="153"/>
-      <c r="L4" t="s">
+      <c r="C4" s="185"/>
+      <c r="D4" s="185"/>
+      <c r="E4" s="185"/>
+      <c r="F4" s="185"/>
+      <c r="G4" s="185"/>
+      <c r="L4" s="186" t="s">
         <v>107</v>
       </c>
+      <c r="M4" s="186" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="134" t="s">
+      <c r="C5" s="179" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="123" t="s">
+      <c r="D5" s="132" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="112" t="s">
+      <c r="E5" s="141" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="113"/>
-      <c r="G5" s="113"/>
-      <c r="H5" s="113"/>
-      <c r="I5" s="113"/>
-      <c r="J5" s="113"/>
-      <c r="K5" s="114"/>
+      <c r="F5" s="142"/>
+      <c r="G5" s="142"/>
+      <c r="H5" s="142"/>
+      <c r="I5" s="142"/>
+      <c r="J5" s="142"/>
+      <c r="K5" s="143"/>
       <c r="L5" s="88" t="s">
         <v>6</v>
       </c>
       <c r="M5" s="66"/>
     </row>
     <row r="6" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="133"/>
-      <c r="C6" s="135"/>
-      <c r="D6" s="136"/>
+      <c r="B6" s="178"/>
+      <c r="C6" s="180"/>
+      <c r="D6" s="181"/>
       <c r="E6" s="16" t="s">
         <v>67</v>
       </c>
@@ -4698,69 +4710,77 @@
       <c r="B7" s="15">
         <v>1</v>
       </c>
-      <c r="C7" s="171" t="s">
+      <c r="C7" s="110" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="170" t="s">
+      <c r="D7" s="109" t="s">
         <v>100</v>
       </c>
-      <c r="E7" s="169">
+      <c r="E7" s="108">
         <v>1</v>
       </c>
-      <c r="F7" s="169" t="s">
+      <c r="F7" s="108" t="s">
         <v>75</v>
       </c>
-      <c r="G7" s="169" t="s">
+      <c r="G7" s="108" t="s">
         <v>101</v>
       </c>
-      <c r="H7" s="173" t="s">
+      <c r="H7" s="112" t="s">
         <v>73</v>
       </c>
-      <c r="I7" s="169" t="s">
+      <c r="I7" s="108" t="s">
         <v>76</v>
       </c>
       <c r="J7" s="93" t="s">
         <v>78</v>
       </c>
-      <c r="K7" s="175" t="s">
+      <c r="K7" s="113" t="s">
         <v>80</v>
       </c>
-      <c r="L7" s="164"/>
-      <c r="M7" s="66"/>
+      <c r="L7" s="103" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" s="113" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" s="70">
         <v>2</v>
       </c>
-      <c r="C8" s="172" t="s">
+      <c r="C8" s="111" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="170" t="s">
+      <c r="D8" s="109" t="s">
         <v>100</v>
       </c>
-      <c r="E8" s="169">
+      <c r="E8" s="108">
         <v>1</v>
       </c>
-      <c r="F8" s="169" t="s">
+      <c r="F8" s="108" t="s">
         <v>75</v>
       </c>
-      <c r="G8" s="169" t="s">
+      <c r="G8" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="H8" s="169" t="s">
+      <c r="H8" s="108" t="s">
         <v>77</v>
       </c>
-      <c r="I8" s="169" t="s">
+      <c r="I8" s="108" t="s">
         <v>76</v>
       </c>
       <c r="J8" s="93" t="s">
         <v>78</v>
       </c>
-      <c r="K8" s="175" t="s">
+      <c r="K8" s="113" t="s">
         <v>80</v>
       </c>
-      <c r="L8" s="164"/>
-      <c r="M8" s="66"/>
+      <c r="L8" s="113" t="s">
+        <v>80</v>
+      </c>
+      <c r="M8" s="113" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="70">
@@ -4769,7 +4789,7 @@
       <c r="C9" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="170" t="s">
+      <c r="D9" s="109" t="s">
         <v>100</v>
       </c>
       <c r="E9" s="71">
@@ -4781,7 +4801,7 @@
       <c r="G9" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="H9" s="167" t="s">
+      <c r="H9" s="106" t="s">
         <v>82</v>
       </c>
       <c r="I9" s="71" t="s">
@@ -4790,11 +4810,15 @@
       <c r="J9" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="K9" s="166" t="s">
+      <c r="K9" s="105" t="s">
         <v>80</v>
       </c>
-      <c r="L9" s="72"/>
-      <c r="M9" s="66"/>
+      <c r="L9" s="113" t="s">
+        <v>80</v>
+      </c>
+      <c r="M9" s="113" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="10" spans="2:13" s="34" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="70">
@@ -4803,7 +4827,7 @@
       <c r="C10" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="170" t="s">
+      <c r="D10" s="109" t="s">
         <v>100</v>
       </c>
       <c r="E10" s="71">
@@ -4815,7 +4839,7 @@
       <c r="G10" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="167" t="s">
+      <c r="H10" s="106" t="s">
         <v>73</v>
       </c>
       <c r="I10" s="71" t="s">
@@ -4824,11 +4848,15 @@
       <c r="J10" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="K10" s="158" t="s">
+      <c r="K10" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="L10" s="74"/>
-      <c r="M10" s="66"/>
+      <c r="L10" s="103" t="b">
+        <v>1</v>
+      </c>
+      <c r="M10" s="103" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="2:13" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="70">
@@ -4837,7 +4865,7 @@
       <c r="C11" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="170" t="s">
+      <c r="D11" s="109" t="s">
         <v>100</v>
       </c>
       <c r="E11" s="71">
@@ -4849,7 +4877,7 @@
       <c r="G11" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="167" t="s">
+      <c r="H11" s="106" t="s">
         <v>93</v>
       </c>
       <c r="I11" s="71" t="s">
@@ -4858,17 +4886,21 @@
       <c r="J11" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="K11" s="165" t="s">
+      <c r="K11" s="104" t="s">
         <v>80</v>
       </c>
-      <c r="L11" s="74"/>
-      <c r="M11" s="66"/>
+      <c r="L11" s="113" t="s">
+        <v>80</v>
+      </c>
+      <c r="M11" s="113" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="12" spans="2:13" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="70">
         <v>6</v>
       </c>
-      <c r="C12" s="170" t="s">
+      <c r="C12" s="109" t="s">
         <v>100</v>
       </c>
       <c r="D12" s="84" t="s">
@@ -4880,10 +4912,10 @@
       <c r="F12" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="G12" s="167" t="s">
+      <c r="G12" s="106" t="s">
         <v>95</v>
       </c>
-      <c r="H12" s="167" t="s">
+      <c r="H12" s="106" t="s">
         <v>73</v>
       </c>
       <c r="I12" s="71" t="s">
@@ -4892,17 +4924,21 @@
       <c r="J12" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="K12" s="166" t="s">
+      <c r="K12" s="105" t="s">
         <v>80</v>
       </c>
-      <c r="L12" s="74"/>
-      <c r="M12" s="66"/>
+      <c r="L12" s="113" t="s">
+        <v>80</v>
+      </c>
+      <c r="M12" s="113" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="13" spans="2:13" s="35" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="70">
         <v>7</v>
       </c>
-      <c r="C13" s="170" t="s">
+      <c r="C13" s="109" t="s">
         <v>100</v>
       </c>
       <c r="D13" s="84" t="s">
@@ -4917,7 +4953,7 @@
       <c r="G13" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="H13" s="167" t="s">
+      <c r="H13" s="106" t="s">
         <v>73</v>
       </c>
       <c r="I13" s="71" t="s">
@@ -4926,16 +4962,21 @@
       <c r="J13" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="K13" s="158" t="s">
+      <c r="K13" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="L13" s="74"/>
+      <c r="L13" s="103" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" s="103" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="70">
         <v>8</v>
       </c>
-      <c r="C14" s="170" t="s">
+      <c r="C14" s="109" t="s">
         <v>100</v>
       </c>
       <c r="D14" s="84" t="s">
@@ -4950,7 +4991,7 @@
       <c r="G14" s="71" t="s">
         <v>98</v>
       </c>
-      <c r="H14" s="167" t="s">
+      <c r="H14" s="106" t="s">
         <v>73</v>
       </c>
       <c r="I14" s="71" t="s">
@@ -4959,17 +5000,21 @@
       <c r="J14" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="K14" s="158" t="s">
+      <c r="K14" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="L14" s="74"/>
-      <c r="M14" s="66"/>
+      <c r="L14" s="103" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" s="103" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="70">
         <v>9</v>
       </c>
-      <c r="C15" s="170" t="s">
+      <c r="C15" s="109" t="s">
         <v>100</v>
       </c>
       <c r="D15" s="84" t="s">
@@ -4981,10 +5026,10 @@
       <c r="F15" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="167" t="s">
-        <v>99</v>
-      </c>
-      <c r="H15" s="167" t="s">
+      <c r="G15" s="106" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" s="106" t="s">
         <v>73</v>
       </c>
       <c r="I15" s="71" t="s">
@@ -4993,11 +5038,15 @@
       <c r="J15" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="K15" s="165" t="s">
+      <c r="K15" s="104" t="s">
         <v>80</v>
       </c>
-      <c r="L15" s="74"/>
-      <c r="M15" s="66"/>
+      <c r="L15" s="113" t="s">
+        <v>80</v>
+      </c>
+      <c r="M15" s="113" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="70">
@@ -5274,119 +5323,127 @@
       <c r="L33" s="4"/>
     </row>
     <row r="34" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C34" s="144"/>
-      <c r="D34" s="144"/>
-      <c r="E34" s="145"/>
+      <c r="C34" s="171"/>
+      <c r="D34" s="171"/>
+      <c r="E34" s="182"/>
       <c r="F34" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G34" s="146" t="s">
+      <c r="G34" s="169" t="s">
         <v>23</v>
       </c>
-      <c r="H34" s="147"/>
-      <c r="I34" s="147"/>
-      <c r="J34" s="144"/>
-      <c r="K34" s="179"/>
-      <c r="L34" s="185" t="s">
+      <c r="H34" s="170"/>
+      <c r="I34" s="170"/>
+      <c r="J34" s="171"/>
+      <c r="K34" s="172"/>
+      <c r="L34" s="175" t="s">
         <v>25</v>
       </c>
-      <c r="M34" s="182"/>
-      <c r="N34" s="183"/>
+      <c r="M34" s="176"/>
+      <c r="N34" s="177"/>
     </row>
     <row r="35" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="66"/>
-      <c r="C35" s="143" t="s">
+      <c r="C35" s="183" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="143" t="s">
+      <c r="D35" s="183" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="142" t="s">
+      <c r="E35" s="158" t="s">
         <v>21</v>
       </c>
-      <c r="F35" s="141" t="s">
+      <c r="F35" s="168" t="s">
         <v>20</v>
       </c>
-      <c r="G35" s="148" t="s">
+      <c r="G35" s="173" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="149"/>
-      <c r="I35" s="177" t="s">
+      <c r="H35" s="162"/>
+      <c r="I35" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="J35" s="149"/>
-      <c r="K35" s="142" t="s">
+      <c r="J35" s="162"/>
+      <c r="K35" s="158" t="s">
         <v>33</v>
       </c>
-      <c r="L35" s="180" t="s">
+      <c r="L35" s="165" t="s">
         <v>22</v>
       </c>
-      <c r="M35" s="181" t="s">
+      <c r="M35" s="167" t="s">
         <v>27</v>
       </c>
-      <c r="N35" s="140" t="s">
+      <c r="N35" s="157" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" s="66"/>
-      <c r="C36" s="143"/>
-      <c r="D36" s="143"/>
-      <c r="E36" s="142"/>
-      <c r="F36" s="141"/>
-      <c r="G36" s="150"/>
-      <c r="H36" s="151"/>
-      <c r="I36" s="178"/>
-      <c r="J36" s="151"/>
-      <c r="K36" s="142"/>
-      <c r="L36" s="139"/>
-      <c r="M36" s="140"/>
-      <c r="N36" s="142"/>
+      <c r="C36" s="183"/>
+      <c r="D36" s="183"/>
+      <c r="E36" s="158"/>
+      <c r="F36" s="168"/>
+      <c r="G36" s="174"/>
+      <c r="H36" s="164"/>
+      <c r="I36" s="163"/>
+      <c r="J36" s="164"/>
+      <c r="K36" s="158"/>
+      <c r="L36" s="166"/>
+      <c r="M36" s="157"/>
+      <c r="N36" s="158"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B37" s="66"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="137"/>
-      <c r="H37" s="138"/>
-      <c r="I37" s="137"/>
-      <c r="J37" s="138"/>
-      <c r="K37" s="25"/>
+      <c r="C37" s="24">
+        <v>8</v>
+      </c>
+      <c r="D37" s="24">
+        <v>1</v>
+      </c>
+      <c r="E37" s="25">
+        <v>1</v>
+      </c>
+      <c r="F37" s="29">
+        <v>1</v>
+      </c>
+      <c r="G37" s="159"/>
+      <c r="H37" s="160"/>
+      <c r="I37" s="159"/>
+      <c r="J37" s="160"/>
+      <c r="K37" s="25">
+        <v>0</v>
+      </c>
       <c r="L37" s="28"/>
       <c r="M37" s="27"/>
-      <c r="N37" s="25"/>
+      <c r="N37" s="25">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B38" s="66"/>
-      <c r="C38" s="184"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="137"/>
-      <c r="H38" s="138"/>
-      <c r="I38" s="137"/>
-      <c r="J38" s="138"/>
+      <c r="C38" s="115">
+        <v>9</v>
+      </c>
+      <c r="D38" s="27">
+        <v>0</v>
+      </c>
+      <c r="E38" s="25">
+        <v>0</v>
+      </c>
+      <c r="F38" s="29">
+        <v>0</v>
+      </c>
+      <c r="G38" s="159"/>
+      <c r="H38" s="160"/>
+      <c r="I38" s="159"/>
+      <c r="J38" s="160"/>
       <c r="K38" s="28"/>
-      <c r="L38" s="176"/>
+      <c r="L38" s="114"/>
       <c r="M38" s="27"/>
       <c r="N38" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="N35:N36"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I35:J36"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="L35:L36"/>
-    <mergeCell ref="M35:M36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="G35:H36"/>
-    <mergeCell ref="L34:N34"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
@@ -5398,6 +5455,18 @@
     <mergeCell ref="E5:K5"/>
     <mergeCell ref="E35:E36"/>
     <mergeCell ref="C3:G4"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="G35:H36"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="N35:N36"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I35:J36"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="L35:L36"/>
+    <mergeCell ref="M35:M36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5406,21 +5475,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A33786056CB34C49BCEFA0219ACF09AA" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fe1a16f605cb49944c1e91188c54d23f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="63f82232-4b4a-4992-a008-0c2680091aa8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8c3ae1477633211a0ddb73f406e1224d" ns2:_="">
     <xsd:import namespace="63f82232-4b4a-4992-a008-0c2680091aa8"/>
@@ -5584,24 +5638,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B88DD952-A6CF-436F-8B36-51E413798B79}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73A5BE66-B540-4CCE-B0F4-199F4D574EF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E0B58DA-A86C-4275-91CE-56836C8F6B2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5617,4 +5669,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73A5BE66-B540-4CCE-B0F4-199F4D574EF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B88DD952-A6CF-436F-8B36-51E413798B79}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>